<commit_message>
First version is complete - Purchase transactions are being stored. - Sales are being stored - Customers are being handled - Inventory is being updated
</commit_message>
<xml_diff>
--- a/assets/invoice2.xlsx
+++ b/assets/invoice2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28270B1F-DF89-46E5-9C19-0B23D7113C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B165A3F9-278C-4476-958B-2129EC473A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Description</t>
   </si>
@@ -89,6 +89,18 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Ghussia Shopper House</t>
+  </si>
+  <si>
+    <t>+92 332 835 9701</t>
+  </si>
+  <si>
+    <t>Please make all checks payable to Ghussia Shopper House</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +114,7 @@
     <numFmt numFmtId="167" formatCode="_([$PKR]\ * #,##0.00_);_([$PKR]\ * \(#,##0.00\);_([$PKR]\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_([$PKR]\ * #,##0_);_([$PKR]\ * \(#,##0\);_([$PKR]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.749961851863155"/>
@@ -289,6 +301,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="2" tint="-0.749961851863155"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="36"/>
       <color theme="2" tint="-0.749961851863155"/>
       <name val="Garamond"/>
       <family val="1"/>
@@ -432,7 +452,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -580,14 +600,20 @@
     <xf numFmtId="168" fontId="25" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1144,211 +1170,6 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9567301F-78A9-415C-B049-F8670113664A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="367611"/>
-          <a:ext cx="5490820" cy="2148840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114532</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1101436</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>560942</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC7EFB7F-8C61-44E8-B0C8-49AE23A83C52}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19050" y="3429232"/>
-          <a:ext cx="2217766" cy="842650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>428626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>211859</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>680371</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CAAA012-C032-44D4-9A6F-3998B59A83DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2386966"/>
-          <a:ext cx="5141999" cy="2004345"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>146739</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>126454</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5970082F-56F4-498C-83AE-C7AD9C8E1A09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4490085" y="689611"/>
-          <a:ext cx="3802434" cy="800823"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>367611</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>560680</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>558111</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C857B2ED-6961-4115-9D55-2E539F8989BB}"/>
             </a:ext>
           </a:extLst>
@@ -1826,7 +1647,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="67" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="33.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1842,28 +1663,30 @@
   <sheetData>
     <row r="1" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="57.9" customHeight="1" x14ac:dyDescent="1.1000000000000001">
-      <c r="A2" s="2"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
@@ -2011,40 +1834,38 @@
         <v>15</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
+      <c r="A20" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C4"/>
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D4"/>
   </mergeCells>
-  <dataValidations count="28">
+  <dataValidations count="27">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The total amount is automatically calculated in this cell" sqref="F18" xr:uid="{0EB0BD25-F164-496C-B660-7CF40AEF7FF3}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the deposit amount, if any" sqref="D18" xr:uid="{4F1AB6AD-0BD8-4D04-9394-2E86684C3CB0}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter tax rate in this cell" sqref="D16" xr:uid="{AEE2507C-80A1-4F12-A888-72439C903102}"/>
@@ -2071,7 +1892,6 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter customer phone number in the cell at right" sqref="E11" xr:uid="{E02A5A6F-8347-4655-A391-756DBD4FAA16}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter customer phone number in this cell" sqref="F11" xr:uid="{ADDEC186-40CE-4366-9D85-9E5D311BA6BA}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Update this cell with your company's email address and website" sqref="A21:F21" xr:uid="{A2184B07-EC4E-40DE-9E46-1CA194FC585F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Modify company name in this cell and the cell below. Enter company address, phone, fax, and email in cells B7 to B11. Enter Billing details in cells G3 to G11." sqref="B2:C2" xr:uid="{DB6F9552-CC87-4242-8BA4-418476BAD0C8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Company name is automatically appended in this cell" sqref="A20:F20" xr:uid="{9037BC3F-22DC-493A-8191-E0D847F633E9}"/>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2080,9 +1900,8 @@
   <headerFooter differentFirst="1" alignWithMargins="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2113,16 +1932,16 @@
     <row r="1" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="57.9" customHeight="1" x14ac:dyDescent="1.1000000000000001">
       <c r="A2" s="2"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="7"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
@@ -2131,8 +1950,8 @@
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="10"/>
       <c r="E4" s="8" t="s">
         <v>11</v>
@@ -2287,24 +2106,24 @@
       <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
     </row>
     <row r="21" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>

</xml_diff>